<commit_message>
Initial refactoring (delete unnecessary files)
</commit_message>
<xml_diff>
--- a/commands/test.xlsx
+++ b/commands/test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbkoh\Documents\ipython\quiver_control_framework\commands\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\honam\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12720" windowHeight="7950"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="14415" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>zone</t>
   </si>
@@ -35,9 +35,6 @@
     <t>actuator_type</t>
   </si>
   <si>
-    <t>RM-4132</t>
-  </si>
-  <si>
     <t>uuid</t>
   </si>
   <si>
@@ -62,7 +59,13 @@
     <t>Occupied Command</t>
   </si>
   <si>
-    <t>9/25/2015 16:47:15</t>
+    <t>11/10/2015 14:35:15</t>
+  </si>
+  <si>
+    <t>11/10/2015 14:50:15</t>
+  </si>
+  <si>
+    <t>RM-2109</t>
   </si>
 </sst>
 </file>
@@ -381,24 +384,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="3" max="3" width="15.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -407,32 +411,46 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <v>-1</v>
       </c>
     </row>

</xml_diff>